<commit_message>
updated scoring to version 5.4
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" activeTab="3"/>
+    <workbookView xWindow="-5010" yWindow="45" windowWidth="21075" windowHeight="8250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs" sheetId="9" r:id="rId1"/>
@@ -1313,11 +1313,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="125934080"/>
-        <c:axId val="124817344"/>
+        <c:axId val="115018752"/>
+        <c:axId val="113283584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125934080"/>
+        <c:axId val="115018752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124817344"/>
+        <c:crossAx val="113283584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +1358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124817344"/>
+        <c:axId val="113283584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1370,7 +1370,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125934080"/>
+        <c:crossAx val="115018752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1518,8 +1518,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132892672"/>
-        <c:axId val="132585664"/>
+        <c:axId val="130796544"/>
+        <c:axId val="127851264"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1631,11 +1631,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132893696"/>
-        <c:axId val="132586240"/>
+        <c:axId val="130797056"/>
+        <c:axId val="127851840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132892672"/>
+        <c:axId val="130796544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,14 +1661,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132585664"/>
+        <c:crossAx val="127851264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1676,7 +1675,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132585664"/>
+        <c:axId val="127851264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1700,19 +1699,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132892672"/>
+        <c:crossAx val="130796544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132586240"/>
+        <c:axId val="127851840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,19 +1736,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132893696"/>
+        <c:crossAx val="130797056"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="132893696"/>
+        <c:axId val="130797056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,7 +1757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132586240"/>
+        <c:crossAx val="127851840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1770,7 +1767,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1928,11 +1924,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66221568"/>
-        <c:axId val="79271552"/>
+        <c:axId val="130536960"/>
+        <c:axId val="130377408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66221568"/>
+        <c:axId val="130536960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1965,7 +1961,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79271552"/>
+        <c:crossAx val="130377408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1973,7 +1969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79271552"/>
+        <c:axId val="130377408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2009,7 +2005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66221568"/>
+        <c:crossAx val="130536960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2158,8 +2154,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66211328"/>
-        <c:axId val="137614400"/>
+        <c:axId val="130537472"/>
+        <c:axId val="130379136"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2271,11 +2267,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90850304"/>
-        <c:axId val="137614976"/>
+        <c:axId val="130538496"/>
+        <c:axId val="130379712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="66211328"/>
+        <c:axId val="130537472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2308,7 +2304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137614400"/>
+        <c:crossAx val="130379136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2316,7 +2312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137614400"/>
+        <c:axId val="130379136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2347,12 +2343,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66211328"/>
+        <c:crossAx val="130537472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137614976"/>
+        <c:axId val="130379712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2385,12 +2381,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90850304"/>
+        <c:crossAx val="130538496"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="90850304"/>
+        <c:axId val="130538496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137614976"/>
+        <c:crossAx val="130379712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2564,8 +2560,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133304320"/>
-        <c:axId val="132670592"/>
+        <c:axId val="130854912"/>
+        <c:axId val="130382016"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2644,11 +2640,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128047104"/>
-        <c:axId val="132671168"/>
+        <c:axId val="127920640"/>
+        <c:axId val="130382592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133304320"/>
+        <c:axId val="130854912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2672,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132670592"/>
+        <c:crossAx val="130382016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2684,7 +2680,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132670592"/>
+        <c:axId val="130382016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2715,12 +2711,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133304320"/>
+        <c:crossAx val="130854912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132671168"/>
+        <c:axId val="130382592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2748,12 +2744,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128047104"/>
+        <c:crossAx val="127920640"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="128047104"/>
+        <c:axId val="127920640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2762,7 +2758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132671168"/>
+        <c:crossAx val="130382592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2913,8 +2909,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133305856"/>
-        <c:axId val="132673472"/>
+        <c:axId val="130856448"/>
+        <c:axId val="131114112"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3026,11 +3022,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133306880"/>
-        <c:axId val="132674048"/>
+        <c:axId val="130857472"/>
+        <c:axId val="131114688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133305856"/>
+        <c:axId val="130856448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3062,7 +3058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132673472"/>
+        <c:crossAx val="131114112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3070,7 +3066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132673472"/>
+        <c:axId val="131114112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3100,12 +3096,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133305856"/>
+        <c:crossAx val="130856448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132674048"/>
+        <c:axId val="131114688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,12 +3133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133306880"/>
+        <c:crossAx val="130857472"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="133306880"/>
+        <c:axId val="130857472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3152,7 +3148,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132674048"/>
+        <c:crossAx val="131114688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3315,8 +3311,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132952064"/>
-        <c:axId val="132676352"/>
+        <c:axId val="131047424"/>
+        <c:axId val="131116992"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3440,11 +3436,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133307392"/>
-        <c:axId val="132676928"/>
+        <c:axId val="130857984"/>
+        <c:axId val="131117568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132952064"/>
+        <c:axId val="131047424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3476,7 +3472,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132676352"/>
+        <c:crossAx val="131116992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3484,7 +3480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132676352"/>
+        <c:axId val="131116992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3519,12 +3515,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132952064"/>
+        <c:crossAx val="131047424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132676928"/>
+        <c:axId val="131117568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3552,12 +3548,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133307392"/>
+        <c:crossAx val="130857984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="133307392"/>
+        <c:axId val="130857984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3567,7 +3563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132676928"/>
+        <c:crossAx val="131117568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3718,8 +3714,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132953600"/>
-        <c:axId val="133195456"/>
+        <c:axId val="131049984"/>
+        <c:axId val="131119872"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3831,11 +3827,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132954624"/>
-        <c:axId val="133196032"/>
+        <c:axId val="131051008"/>
+        <c:axId val="131120448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132953600"/>
+        <c:axId val="131049984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3867,7 +3863,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133195456"/>
+        <c:crossAx val="131119872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3875,7 +3871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133195456"/>
+        <c:axId val="131119872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3905,12 +3901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132953600"/>
+        <c:crossAx val="131049984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133196032"/>
+        <c:axId val="131120448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3942,12 +3938,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132954624"/>
+        <c:crossAx val="131051008"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="132954624"/>
+        <c:axId val="131051008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3957,7 +3953,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133196032"/>
+        <c:crossAx val="131120448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4120,8 +4116,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133156864"/>
-        <c:axId val="133198336"/>
+        <c:axId val="133425152"/>
+        <c:axId val="133465792"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4245,11 +4241,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132955136"/>
-        <c:axId val="133198912"/>
+        <c:axId val="133424128"/>
+        <c:axId val="133466368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133156864"/>
+        <c:axId val="133425152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4281,7 +4277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133198336"/>
+        <c:crossAx val="133465792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4289,7 +4285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133198336"/>
+        <c:axId val="133465792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4324,12 +4320,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133156864"/>
+        <c:crossAx val="133425152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133198912"/>
+        <c:axId val="133466368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4357,12 +4353,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132955136"/>
+        <c:crossAx val="133424128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="132955136"/>
+        <c:axId val="133424128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4372,7 +4368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133198912"/>
+        <c:crossAx val="133466368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4523,8 +4519,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133160448"/>
-        <c:axId val="133201216"/>
+        <c:axId val="133426688"/>
+        <c:axId val="133468672"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4636,11 +4632,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133579264"/>
-        <c:axId val="133398528"/>
+        <c:axId val="134722048"/>
+        <c:axId val="133469248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133160448"/>
+        <c:axId val="133426688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4672,7 +4668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133201216"/>
+        <c:crossAx val="133468672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4680,7 +4676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133201216"/>
+        <c:axId val="133468672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4710,12 +4706,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133160448"/>
+        <c:crossAx val="133426688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133398528"/>
+        <c:axId val="133469248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4747,12 +4743,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133579264"/>
+        <c:crossAx val="134722048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="133579264"/>
+        <c:axId val="134722048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4762,7 +4758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133398528"/>
+        <c:crossAx val="133469248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4928,11 +4924,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133580800"/>
-        <c:axId val="133400832"/>
+        <c:axId val="134723584"/>
+        <c:axId val="133471552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133580800"/>
+        <c:axId val="134723584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4964,7 +4960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133400832"/>
+        <c:crossAx val="133471552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4972,7 +4968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133400832"/>
+        <c:axId val="133471552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5007,7 +5003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133580800"/>
+        <c:crossAx val="134723584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5085,7 +5081,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5699,11 +5694,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127832064"/>
-        <c:axId val="124819648"/>
+        <c:axId val="117608448"/>
+        <c:axId val="113285888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127832064"/>
+        <c:axId val="117608448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5730,14 +5725,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124819648"/>
+        <c:crossAx val="113285888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5745,7 +5739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124819648"/>
+        <c:axId val="113285888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5757,14 +5751,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127832064"/>
+        <c:crossAx val="117608448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5906,8 +5899,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133582336"/>
-        <c:axId val="133402560"/>
+        <c:axId val="134724608"/>
+        <c:axId val="134653056"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6019,11 +6012,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133800448"/>
-        <c:axId val="133403136"/>
+        <c:axId val="134725120"/>
+        <c:axId val="134653632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133582336"/>
+        <c:axId val="134724608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6055,7 +6048,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133402560"/>
+        <c:crossAx val="134653056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6063,7 +6056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133402560"/>
+        <c:axId val="134653056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -6093,12 +6086,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133582336"/>
+        <c:crossAx val="134724608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133403136"/>
+        <c:axId val="134653632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6130,12 +6123,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133800448"/>
+        <c:crossAx val="134725120"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="133800448"/>
+        <c:axId val="134725120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6145,7 +6138,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133403136"/>
+        <c:crossAx val="134653632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6311,11 +6304,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133801472"/>
-        <c:axId val="133405440"/>
+        <c:axId val="134985216"/>
+        <c:axId val="134655936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133801472"/>
+        <c:axId val="134985216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6347,7 +6340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133405440"/>
+        <c:crossAx val="134655936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6355,7 +6348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133405440"/>
+        <c:axId val="134655936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -6390,7 +6383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133801472"/>
+        <c:crossAx val="134985216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6538,8 +6531,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133801984"/>
-        <c:axId val="133718592"/>
+        <c:axId val="134985728"/>
+        <c:axId val="134657664"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6651,11 +6644,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133803008"/>
-        <c:axId val="133719168"/>
+        <c:axId val="134986752"/>
+        <c:axId val="134658240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133801984"/>
+        <c:axId val="134985728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6687,7 +6680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133718592"/>
+        <c:crossAx val="134657664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6695,7 +6688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133718592"/>
+        <c:axId val="134657664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -6725,12 +6718,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133801984"/>
+        <c:crossAx val="134985728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133719168"/>
+        <c:axId val="134658240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6762,12 +6755,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133803008"/>
+        <c:crossAx val="134986752"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="133803008"/>
+        <c:axId val="134986752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6777,7 +6770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133719168"/>
+        <c:crossAx val="134658240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6940,8 +6933,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135274496"/>
-        <c:axId val="133721472"/>
+        <c:axId val="137248768"/>
+        <c:axId val="136159808"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7065,11 +7058,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133159424"/>
-        <c:axId val="133722048"/>
+        <c:axId val="133423616"/>
+        <c:axId val="136160384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135274496"/>
+        <c:axId val="137248768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7101,7 +7094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133721472"/>
+        <c:crossAx val="136159808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7109,7 +7102,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133721472"/>
+        <c:axId val="136159808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -7144,12 +7137,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135274496"/>
+        <c:crossAx val="137248768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133722048"/>
+        <c:axId val="136160384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7177,12 +7170,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133159424"/>
+        <c:crossAx val="133423616"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="133159424"/>
+        <c:axId val="133423616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7192,7 +7185,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133722048"/>
+        <c:crossAx val="136160384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7343,8 +7336,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135276032"/>
-        <c:axId val="133724352"/>
+        <c:axId val="137250304"/>
+        <c:axId val="136162688"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7456,11 +7449,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135277056"/>
-        <c:axId val="133724928"/>
+        <c:axId val="137251328"/>
+        <c:axId val="136163264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135276032"/>
+        <c:axId val="137250304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7492,7 +7485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133724352"/>
+        <c:crossAx val="136162688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7500,7 +7493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133724352"/>
+        <c:axId val="136162688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -7530,12 +7523,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135276032"/>
+        <c:crossAx val="137250304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133724928"/>
+        <c:axId val="136163264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7567,12 +7560,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135277056"/>
+        <c:crossAx val="137251328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="135277056"/>
+        <c:axId val="137251328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7582,7 +7575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133724928"/>
+        <c:crossAx val="136163264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7745,8 +7738,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134103040"/>
-        <c:axId val="134194304"/>
+        <c:axId val="138600448"/>
+        <c:axId val="136165568"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -7870,11 +7863,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135277568"/>
-        <c:axId val="134194880"/>
+        <c:axId val="137251840"/>
+        <c:axId val="136166144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134103040"/>
+        <c:axId val="138600448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7906,7 +7899,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134194304"/>
+        <c:crossAx val="136165568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7914,7 +7907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134194304"/>
+        <c:axId val="136165568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -7949,12 +7942,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134103040"/>
+        <c:crossAx val="138600448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134194880"/>
+        <c:axId val="136166144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7982,12 +7975,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135277568"/>
+        <c:crossAx val="137251840"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="135277568"/>
+        <c:axId val="137251840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7997,7 +7990,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134194880"/>
+        <c:crossAx val="136166144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8148,8 +8141,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134104576"/>
-        <c:axId val="134197184"/>
+        <c:axId val="138601984"/>
+        <c:axId val="138462336"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8261,11 +8254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134105600"/>
-        <c:axId val="134197760"/>
+        <c:axId val="138603008"/>
+        <c:axId val="138462912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="134104576"/>
+        <c:axId val="138601984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8297,7 +8290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134197184"/>
+        <c:crossAx val="138462336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8305,7 +8298,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134197184"/>
+        <c:axId val="138462336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -8335,12 +8328,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134104576"/>
+        <c:crossAx val="138601984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134197760"/>
+        <c:axId val="138462912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8372,12 +8365,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134105600"/>
+        <c:crossAx val="138603008"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="134105600"/>
+        <c:axId val="138603008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8387,7 +8380,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134197760"/>
+        <c:crossAx val="138462912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8550,8 +8543,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135663616"/>
-        <c:axId val="134199488"/>
+        <c:axId val="138870784"/>
+        <c:axId val="138464640"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -8675,11 +8668,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="134106112"/>
-        <c:axId val="134200064"/>
+        <c:axId val="138603520"/>
+        <c:axId val="138465216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135663616"/>
+        <c:axId val="138870784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8711,7 +8704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134199488"/>
+        <c:crossAx val="138464640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8719,7 +8712,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134199488"/>
+        <c:axId val="138464640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -8754,12 +8747,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135663616"/>
+        <c:crossAx val="138870784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134200064"/>
+        <c:axId val="138465216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8787,12 +8780,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134106112"/>
+        <c:crossAx val="138603520"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="134106112"/>
+        <c:axId val="138603520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8802,7 +8795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134200064"/>
+        <c:crossAx val="138465216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8953,8 +8946,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135665152"/>
-        <c:axId val="135365760"/>
+        <c:axId val="138872320"/>
+        <c:axId val="138467520"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9066,11 +9059,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135666176"/>
-        <c:axId val="135366336"/>
+        <c:axId val="138873344"/>
+        <c:axId val="138468096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135665152"/>
+        <c:axId val="138872320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9102,7 +9095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135365760"/>
+        <c:crossAx val="138467520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9110,7 +9103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135365760"/>
+        <c:axId val="138467520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -9140,12 +9133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135665152"/>
+        <c:crossAx val="138872320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135366336"/>
+        <c:axId val="138468096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9177,12 +9170,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135666176"/>
+        <c:crossAx val="138873344"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="135666176"/>
+        <c:axId val="138873344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9192,7 +9185,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135366336"/>
+        <c:crossAx val="138468096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9355,8 +9348,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135532544"/>
-        <c:axId val="135368064"/>
+        <c:axId val="138797056"/>
+        <c:axId val="139395648"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9480,11 +9473,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135666688"/>
-        <c:axId val="135368640"/>
+        <c:axId val="138873856"/>
+        <c:axId val="139396224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135532544"/>
+        <c:axId val="138797056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9516,7 +9509,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135368064"/>
+        <c:crossAx val="139395648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9524,7 +9517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135368064"/>
+        <c:axId val="139395648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -9559,12 +9552,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135532544"/>
+        <c:crossAx val="138797056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135368640"/>
+        <c:axId val="139396224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9592,12 +9585,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135666688"/>
+        <c:crossAx val="138873856"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="135666688"/>
+        <c:axId val="138873856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9607,7 +9600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135368640"/>
+        <c:crossAx val="139396224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9661,7 +9654,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -10314,11 +10306,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127833088"/>
-        <c:axId val="128148032"/>
+        <c:axId val="117609472"/>
+        <c:axId val="127771776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127833088"/>
+        <c:axId val="117609472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10345,14 +10337,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128148032"/>
+        <c:crossAx val="127771776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10360,7 +10351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128148032"/>
+        <c:axId val="127771776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10383,21 +10374,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127833088"/>
+        <c:crossAx val="117609472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -10539,8 +10528,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135534080"/>
-        <c:axId val="135370944"/>
+        <c:axId val="138798592"/>
+        <c:axId val="139398528"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -10652,11 +10641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135535104"/>
-        <c:axId val="135371520"/>
+        <c:axId val="138799616"/>
+        <c:axId val="139399104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="135534080"/>
+        <c:axId val="138798592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10688,7 +10677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135370944"/>
+        <c:crossAx val="139398528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10696,7 +10685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135370944"/>
+        <c:axId val="139398528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -10726,12 +10715,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135534080"/>
+        <c:crossAx val="138798592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135371520"/>
+        <c:axId val="139399104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10763,12 +10752,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135535104"/>
+        <c:crossAx val="138799616"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="135535104"/>
+        <c:axId val="138799616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10778,7 +10767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135371520"/>
+        <c:crossAx val="139399104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10941,8 +10930,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137035776"/>
-        <c:axId val="136970816"/>
+        <c:axId val="139538432"/>
+        <c:axId val="139400832"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11066,11 +11055,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="135535616"/>
-        <c:axId val="136971392"/>
+        <c:axId val="138800128"/>
+        <c:axId val="139401408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137035776"/>
+        <c:axId val="139538432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11102,7 +11091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136970816"/>
+        <c:crossAx val="139400832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11110,7 +11099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136970816"/>
+        <c:axId val="139400832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11145,12 +11134,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137035776"/>
+        <c:crossAx val="139538432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136971392"/>
+        <c:axId val="139401408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11178,12 +11167,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135535616"/>
+        <c:crossAx val="138800128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="135535616"/>
+        <c:axId val="138800128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11193,7 +11182,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136971392"/>
+        <c:crossAx val="139401408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11344,8 +11333,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137037312"/>
-        <c:axId val="136973696"/>
+        <c:axId val="139540992"/>
+        <c:axId val="139452992"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11457,11 +11446,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137038336"/>
-        <c:axId val="136974272"/>
+        <c:axId val="139542016"/>
+        <c:axId val="139453568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137037312"/>
+        <c:axId val="139540992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11493,7 +11482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136973696"/>
+        <c:crossAx val="139452992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11501,7 +11490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136973696"/>
+        <c:axId val="139452992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11531,12 +11520,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137037312"/>
+        <c:crossAx val="139540992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136974272"/>
+        <c:axId val="139453568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11568,12 +11557,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137038336"/>
+        <c:crossAx val="139542016"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="137038336"/>
+        <c:axId val="139542016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11583,7 +11572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136974272"/>
+        <c:crossAx val="139453568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11746,8 +11735,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137121792"/>
-        <c:axId val="136976000"/>
+        <c:axId val="139192320"/>
+        <c:axId val="139455296"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -11871,11 +11860,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137038848"/>
-        <c:axId val="136976576"/>
+        <c:axId val="139191296"/>
+        <c:axId val="139455872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137121792"/>
+        <c:axId val="139192320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11907,7 +11896,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136976000"/>
+        <c:crossAx val="139455296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11915,7 +11904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136976000"/>
+        <c:axId val="139455296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -11950,12 +11939,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137121792"/>
+        <c:crossAx val="139192320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="136976576"/>
+        <c:axId val="139455872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11983,12 +11972,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137038848"/>
+        <c:crossAx val="139191296"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="137038848"/>
+        <c:axId val="139191296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11998,7 +11987,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136976576"/>
+        <c:crossAx val="139455872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12149,8 +12138,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137125376"/>
-        <c:axId val="137028160"/>
+        <c:axId val="139193856"/>
+        <c:axId val="139459328"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12262,11 +12251,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137671168"/>
-        <c:axId val="137028736"/>
+        <c:axId val="139342336"/>
+        <c:axId val="139459904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137125376"/>
+        <c:axId val="139193856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12298,7 +12287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137028160"/>
+        <c:crossAx val="139459328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12306,7 +12295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137028160"/>
+        <c:axId val="139459328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -12336,12 +12325,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137125376"/>
+        <c:crossAx val="139193856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137028736"/>
+        <c:axId val="139459904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12373,12 +12362,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137671168"/>
+        <c:crossAx val="139342336"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="137671168"/>
+        <c:axId val="139342336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12388,7 +12377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137028736"/>
+        <c:crossAx val="139459904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12551,8 +12540,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137672704"/>
-        <c:axId val="137030464"/>
+        <c:axId val="139343872"/>
+        <c:axId val="134546560"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12631,11 +12620,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137124864"/>
-        <c:axId val="137031040"/>
+        <c:axId val="139342848"/>
+        <c:axId val="134547136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137672704"/>
+        <c:axId val="139343872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12667,7 +12656,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137030464"/>
+        <c:crossAx val="134546560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12675,7 +12664,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137030464"/>
+        <c:axId val="134546560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -12710,12 +12699,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137672704"/>
+        <c:crossAx val="139343872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137031040"/>
+        <c:axId val="134547136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12748,12 +12737,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137124864"/>
+        <c:crossAx val="139342848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="137124864"/>
+        <c:axId val="139342848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12762,7 +12751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137031040"/>
+        <c:crossAx val="134547136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12913,8 +12902,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137445376"/>
-        <c:axId val="137034496"/>
+        <c:axId val="139722752"/>
+        <c:axId val="134549440"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12987,11 +12976,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137446400"/>
-        <c:axId val="137035072"/>
+        <c:axId val="139723776"/>
+        <c:axId val="134550016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137445376"/>
+        <c:axId val="139722752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13023,7 +13012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137034496"/>
+        <c:crossAx val="134549440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13031,7 +13020,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137034496"/>
+        <c:axId val="134549440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -13061,12 +13050,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137445376"/>
+        <c:crossAx val="139722752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137035072"/>
+        <c:axId val="134550016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13098,12 +13087,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137446400"/>
+        <c:crossAx val="139723776"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="137446400"/>
+        <c:axId val="139723776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13112,7 +13101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137035072"/>
+        <c:crossAx val="134550016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13487,11 +13476,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127833600"/>
-        <c:axId val="128150336"/>
+        <c:axId val="117610496"/>
+        <c:axId val="127774080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127833600"/>
+        <c:axId val="117610496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13524,7 +13513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128150336"/>
+        <c:crossAx val="127774080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13532,7 +13521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128150336"/>
+        <c:axId val="127774080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -13544,7 +13533,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127833600"/>
+        <c:crossAx val="117610496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13622,7 +13611,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -14058,11 +14046,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127835648"/>
-        <c:axId val="128152064"/>
+        <c:axId val="117612032"/>
+        <c:axId val="127775808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127835648"/>
+        <c:axId val="117612032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14089,14 +14077,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128152064"/>
+        <c:crossAx val="127775808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14104,7 +14091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128152064"/>
+        <c:axId val="127775808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -14116,14 +14103,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127835648"/>
+        <c:crossAx val="117612032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14168,7 +14154,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -14365,11 +14350,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128046592"/>
-        <c:axId val="128153792"/>
+        <c:axId val="127920128"/>
+        <c:axId val="127777536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128046592"/>
+        <c:axId val="127920128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14396,14 +14381,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128153792"/>
+        <c:crossAx val="127777536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14411,7 +14395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128153792"/>
+        <c:axId val="127777536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14434,21 +14418,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128046592"/>
+        <c:crossAx val="127920128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14478,7 +14460,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -14606,11 +14587,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128048640"/>
-        <c:axId val="132579328"/>
+        <c:axId val="68410368"/>
+        <c:axId val="127844928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128048640"/>
+        <c:axId val="68410368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14636,14 +14617,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132579328"/>
+        <c:crossAx val="127844928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14651,7 +14631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132579328"/>
+        <c:axId val="127844928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -14680,21 +14660,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128048640"/>
+        <c:crossAx val="68410368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -14836,8 +14814,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68405760"/>
-        <c:axId val="132581056"/>
+        <c:axId val="68409856"/>
+        <c:axId val="127846656"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14949,11 +14927,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132891136"/>
-        <c:axId val="132581632"/>
+        <c:axId val="130793984"/>
+        <c:axId val="127847232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68405760"/>
+        <c:axId val="68409856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14979,14 +14957,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132581056"/>
+        <c:crossAx val="127846656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14994,7 +14971,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132581056"/>
+        <c:axId val="127846656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -15018,19 +14995,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68405760"/>
+        <c:crossAx val="68409856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132581632"/>
+        <c:axId val="127847232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15056,19 +15032,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132891136"/>
+        <c:crossAx val="130793984"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="132891136"/>
+        <c:axId val="130793984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15078,7 +15053,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132581632"/>
+        <c:crossAx val="127847232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15088,7 +15063,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15118,7 +15092,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -15246,11 +15219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="132892160"/>
-        <c:axId val="132583936"/>
+        <c:axId val="130795520"/>
+        <c:axId val="127849536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="132892160"/>
+        <c:axId val="130795520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15276,14 +15249,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132583936"/>
+        <c:crossAx val="127849536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15291,7 +15263,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132583936"/>
+        <c:axId val="127849536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -15320,21 +15292,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132892160"/>
+        <c:crossAx val="130795520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -34127,8 +34097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>